<commit_message>
atualização cronograma e documentação
</commit_message>
<xml_diff>
--- a/docs/CRONOGRAMA PROJETO STG.xlsx
+++ b/docs/CRONOGRAMA PROJETO STG.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER_NITRO_5\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAA70B2-3F02-4717-A13D-A209F967EC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
@@ -93,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +134,21 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -224,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -239,7 +248,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -252,6 +260,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,73 +588,73 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.109375" customWidth="1"/>
-    <col min="6" max="6" width="37.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="14" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.125" customWidth="1"/>
+    <col min="6" max="6" width="37.5" customWidth="1"/>
+    <col min="7" max="7" width="17.875" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="15.25" customWidth="1"/>
+    <col min="10" max="10" width="16.625" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="14.375" customWidth="1"/>
+    <col min="13" max="14" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" ht="18">
+      <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="18">
+      <c r="A2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" ht="18">
+      <c r="A4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="25.9" customHeight="1">
       <c r="F5" s="4" t="s">
         <v>1</v>
       </c>
@@ -661,68 +671,68 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="35.450000000000003" customHeight="1">
       <c r="F6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="36" customHeight="1">
       <c r="F7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="39" customHeight="1">
       <c r="F8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="39.6" customHeight="1">
       <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="50.45" customHeight="1">
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="10"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="45.6" customHeight="1">
       <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="40.15" customHeight="1">
       <c r="F12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="8"/>
+      <c r="J12" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>